<commit_message>
agragar boton de vista de descarga y subida de archivos de excel y agragar un formulario para subir archivo excel
</commit_message>
<xml_diff>
--- a/public/importaciones/Clientes.xlsx
+++ b/public/importaciones/Clientes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea\Desktop\iconova\sistema-contable-laravel\public\importaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{84537D37-31BA-4F38-AA6D-8F5D53D8C519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DA657-DE94-45AC-B2E2-AE09255AE851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2CA60062-0725-414D-A035-E7C7311FB4AF}"/>
+    <workbookView xWindow="16284" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CA60062-0725-414D-A035-E7C7311FB4AF}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -53,9 +53,6 @@
     <t>magnitud_cliente</t>
   </si>
   <si>
-    <t>tipo_cliebte</t>
-  </si>
-  <si>
     <t>correo</t>
   </si>
   <si>
@@ -93,6 +90,9 @@
   </si>
   <si>
     <t>Contribuyente pequeño</t>
+  </si>
+  <si>
+    <t>tipo_cliente</t>
   </si>
 </sst>
 </file>
@@ -179,13 +179,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -503,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004320B-E9F2-4FA3-BA74-847518F258FE}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,45 +525,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="G7" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -575,7 +571,7 @@
           <x14:formula1>
             <xm:f>tipo_cliente!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
+          <xm:sqref>E2:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1456596D-FF8E-48BB-8D9A-53BD7A29FB8A}">
           <x14:formula1>
@@ -604,17 +600,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -638,22 +634,22 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integracion de la funcion de importar clientes de un archivo excel
</commit_message>
<xml_diff>
--- a/public/importaciones/Clientes.xlsx
+++ b/public/importaciones/Clientes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josea\Desktop\iconova\sistema-contable-laravel\public\importaciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0DA657-DE94-45AC-B2E2-AE09255AE851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E971D6C-35FA-459E-B2AD-9C17779D5EB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16284" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2CA60062-0725-414D-A035-E7C7311FB4AF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{2CA60062-0725-414D-A035-E7C7311FB4AF}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>nombre</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>tipo_cliente</t>
+  </si>
+  <si>
+    <t>nrc</t>
   </si>
 </sst>
 </file>
@@ -124,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -175,17 +178,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -502,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7004320B-E9F2-4FA3-BA74-847518F258FE}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,57 +533,62 @@
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" customWidth="1"/>
-    <col min="7" max="7" width="25.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="4" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>10</v>
       </c>
+      <c r="N1" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
@@ -571,13 +596,13 @@
           <x14:formula1>
             <xm:f>tipo_cliente!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1456596D-FF8E-48BB-8D9A-53BD7A29FB8A}">
           <x14:formula1>
             <xm:f>magnitud_cliente!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F1:F1048576</xm:sqref>
+          <xm:sqref>G1:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>